<commit_message>
BAOCAO VA SUA BAN LE KHUYEN MAI
</commit_message>
<xml_diff>
--- a/ERBus.Api/Upload/BARCODE/TemplateNhapMua.xlsx
+++ b/ERBus.Api/Upload/BARCODE/TemplateNhapMua.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\ERBus\ERBus\ERBus.Api\Upload\BARCODE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\CodeAnhpt\ERBus\ERBus.Api\Upload\BARCODE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,22 +29,22 @@
     <t>Barcode</t>
   </si>
   <si>
-    <t>MaHang</t>
-  </si>
-  <si>
-    <t>TenHang</t>
-  </si>
-  <si>
-    <t>GiaBanBuonVat</t>
-  </si>
-  <si>
-    <t>GiaBanLeVat</t>
-  </si>
-  <si>
-    <t>MaNhaCungCap</t>
-  </si>
-  <si>
-    <t>SoLuong</t>
+    <t>Masieuthi</t>
+  </si>
+  <si>
+    <t>Tenviettat</t>
+  </si>
+  <si>
+    <t>Giabanbuoncovat</t>
+  </si>
+  <si>
+    <t>Giabanlecovat</t>
+  </si>
+  <si>
+    <t>Makhachhang</t>
+  </si>
+  <si>
+    <t>Soluong</t>
   </si>
 </sst>
 </file>
@@ -401,7 +401,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>